<commit_message>
create percentage master list reference data
</commit_message>
<xml_diff>
--- a/data/percentage-master-list.xlsx
+++ b/data/percentage-master-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAP673\weightlifting-nationals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADFD65D-78A1-43F6-A5D3-B0BB1CDE417F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E0F931-5152-49ED-A859-DF4A7D6C2B42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3468,7 +3468,7 @@
         <v>9941160</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" ref="E34:E65" si="8">(C34/D34)*100</f>
+        <f t="shared" ref="E34:E51" si="8">(C34/D34)*100</f>
         <v>1.005918826374387E-4</v>
       </c>
       <c r="F34" s="1">

</xml_diff>

<commit_message>
changer percent to ppm
</commit_message>
<xml_diff>
--- a/data/percentage-master-list.xlsx
+++ b/data/percentage-master-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAP673\weightlifting-nationals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E0F931-5152-49ED-A859-DF4A7D6C2B42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B13330C-DE44-4BCA-8E95-3F6279A3E797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <t>pop</t>
   </si>
   <si>
-    <t>percent</t>
-  </si>
-  <si>
     <t>pop 15</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>pop 17</t>
+  </si>
+  <si>
+    <t>ppm</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1067,34 +1067,34 @@
         <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1">
         <v>2015</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1">
         <v>2016</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="L1" s="1">
         <v>2017</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="O1" s="1">
         <v>2018</v>
@@ -1103,7 +1103,7 @@
         <v>53</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="R1" s="1">
         <v>2019</v>
@@ -1112,7 +1112,7 @@
         <v>53</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>2</v>
@@ -1132,8 +1132,8 @@
         <v>4840037</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" ref="E2:E33" si="0">(C2/D2)*100</f>
-        <v>4.1321998158278545E-5</v>
+        <f>(C2/D2)*1000000</f>
+        <v>0.41321998158278544</v>
       </c>
       <c r="F2" s="1">
         <v>4</v>
@@ -1142,8 +1142,8 @@
         <v>4850858</v>
       </c>
       <c r="H2" s="1">
-        <f>(F2/G2)*100</f>
-        <v>8.245963909889756E-5</v>
+        <f>(F2/G2)*1000000</f>
+        <v>0.82459639098897564</v>
       </c>
       <c r="I2" s="1">
         <v>4</v>
@@ -1152,8 +1152,8 @@
         <v>4860545</v>
       </c>
       <c r="K2" s="1">
-        <f>(I2/J2)*100</f>
-        <v>8.2295298161008697E-5</v>
+        <f>(I2/J2)*1000000</f>
+        <v>0.8229529816100869</v>
       </c>
       <c r="L2" s="1">
         <v>2</v>
@@ -1162,29 +1162,29 @@
         <v>4874747</v>
       </c>
       <c r="N2" s="1">
-        <f>(L2/M2)*100</f>
-        <v>4.1027770261718204E-5</v>
+        <f>(L2/M2)*1000000</f>
+        <v>0.41027770261718199</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
       <c r="P2" s="1">
-        <f t="shared" ref="P2:P33" si="1">M2</f>
+        <f t="shared" ref="P2:P33" si="0">M2</f>
         <v>4874747</v>
       </c>
       <c r="Q2" s="1">
-        <f>(O2/P2)*100</f>
+        <f>(O2/P2)*1000000</f>
         <v>0</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
       <c r="S2" s="1">
-        <f t="shared" ref="S2:S33" si="2">M2</f>
+        <f t="shared" ref="S2:S33" si="1">M2</f>
         <v>4874747</v>
       </c>
       <c r="T2" s="1">
-        <f>(R2/S2)*100</f>
+        <f>(R2/S2)*1000000</f>
         <v>0</v>
       </c>
       <c r="U2" s="1">
@@ -1205,7 +1205,7 @@
         <v>736759</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E3:E51" si="2">(C3/D3)*1000000</f>
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -1215,7 +1215,7 @@
         <v>737979</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H51" si="3">(F3/G3)*100</f>
+        <f t="shared" ref="H3:H51" si="3">(F3/G3)*1000000</f>
         <v>0</v>
       </c>
       <c r="I3" s="1">
@@ -1225,7 +1225,7 @@
         <v>741522</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K51" si="4">(I3/J3)*100</f>
+        <f t="shared" ref="K3:K51" si="4">(I3/J3)*1000000</f>
         <v>0</v>
       </c>
       <c r="L3" s="1">
@@ -1235,29 +1235,29 @@
         <v>739795</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N51" si="5">(L3/M3)*100</f>
-        <v>1.3517258159354955E-4</v>
+        <f t="shared" ref="N3:N51" si="5">(L3/M3)*1000000</f>
+        <v>1.3517258159354957</v>
       </c>
       <c r="O3" s="1">
         <v>1</v>
       </c>
       <c r="P3" s="1">
+        <f t="shared" si="0"/>
+        <v>739795</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:Q51" si="6">(O3/P3)*1000000</f>
+        <v>1.3517258159354957</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
         <f t="shared" si="1"/>
         <v>739795</v>
       </c>
-      <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q51" si="6">(O3/P3)*100</f>
-        <v>1.3517258159354955E-4</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <f t="shared" si="2"/>
-        <v>739795</v>
-      </c>
       <c r="T3" s="1">
-        <f t="shared" ref="T3:T50" si="7">(R3/S3)*100</f>
+        <f t="shared" ref="T3:T51" si="7">(R3/S3)*1000000</f>
         <v>0</v>
       </c>
       <c r="U3" s="1">
@@ -1278,8 +1278,8 @@
         <v>6706435</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6402157032760327E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.6402157032760327</v>
       </c>
       <c r="F4" s="1">
         <v>10</v>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" si="3"/>
-        <v>1.4700992111153614E-4</v>
+        <v>1.4700992111153612</v>
       </c>
       <c r="I4" s="1">
         <v>9</v>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="K4" s="1">
         <f t="shared" si="4"/>
-        <v>1.3027162212197419E-4</v>
+        <v>1.3027162212197418</v>
       </c>
       <c r="L4" s="1">
         <v>6</v>
@@ -1309,29 +1309,29 @@
       </c>
       <c r="N4" s="1">
         <f t="shared" si="5"/>
-        <v>8.5515523205349851E-5</v>
+        <v>0.85515523205349853</v>
       </c>
       <c r="O4" s="1">
         <v>8</v>
       </c>
       <c r="P4" s="1">
+        <f t="shared" si="0"/>
+        <v>7016270</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="6"/>
+        <v>1.1402069760713314</v>
+      </c>
+      <c r="R4" s="1">
+        <v>6</v>
+      </c>
+      <c r="S4" s="1">
         <f t="shared" si="1"/>
         <v>7016270</v>
       </c>
-      <c r="Q4" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1402069760713313E-4</v>
-      </c>
-      <c r="R4" s="1">
-        <v>6</v>
-      </c>
-      <c r="S4" s="1">
-        <f t="shared" si="2"/>
-        <v>7016270</v>
-      </c>
       <c r="T4" s="1">
         <f t="shared" si="7"/>
-        <v>8.5515523205349851E-5</v>
+        <v>0.85515523205349853</v>
       </c>
       <c r="U4" s="1">
         <v>50</v>
@@ -1351,8 +1351,8 @@
         <v>2964800</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>3.3729087965461414E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.33729087965461413</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="3"/>
-        <v>6.7212747838606057E-5</v>
+        <v>0.67212747838606057</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" si="4"/>
-        <v>3.346461501804914E-5</v>
+        <v>0.33464615018049138</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3004279</v>
       </c>
       <c r="Q5" s="1">
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3004279</v>
       </c>
       <c r="T5" s="1">
@@ -1424,8 +1424,8 @@
         <v>38701278</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5244974597479702E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.5244974597479701</v>
       </c>
       <c r="F6" s="1">
         <v>74</v>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="3"/>
-        <v>1.8958587374134195E-4</v>
+        <v>1.8958587374134195</v>
       </c>
       <c r="I6" s="1">
         <v>57</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="4"/>
-        <v>1.4505117456333744E-4</v>
+        <v>1.4505117456333743</v>
       </c>
       <c r="L6" s="1">
         <v>64</v>
@@ -1455,29 +1455,29 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" si="5"/>
-        <v>1.6187510864918182E-4</v>
+        <v>1.6187510864918182</v>
       </c>
       <c r="O6" s="1">
         <v>53</v>
       </c>
       <c r="P6" s="1">
+        <f t="shared" si="0"/>
+        <v>39536653</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="6"/>
+        <v>1.3405282435010368</v>
+      </c>
+      <c r="R6" s="1">
+        <v>57</v>
+      </c>
+      <c r="S6" s="1">
         <f t="shared" si="1"/>
         <v>39536653</v>
       </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="6"/>
-        <v>1.3405282435010368E-4</v>
-      </c>
-      <c r="R6" s="1">
-        <v>57</v>
-      </c>
-      <c r="S6" s="1">
-        <f t="shared" si="2"/>
-        <v>39536653</v>
-      </c>
       <c r="T6" s="1">
         <f t="shared" si="7"/>
-        <v>1.4417001864067754E-4</v>
+        <v>1.4417001864067753</v>
       </c>
       <c r="U6" s="1">
         <v>364</v>
@@ -1497,8 +1497,8 @@
         <v>5342311</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0590340023259599E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.0590340023259599</v>
       </c>
       <c r="F7" s="1">
         <v>28</v>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="3"/>
-        <v>5.1466378209870703E-4</v>
+        <v>5.1466378209870696</v>
       </c>
       <c r="I7" s="1">
         <v>15</v>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="4"/>
-        <v>2.712425894264214E-4</v>
+        <v>2.7124258942642139</v>
       </c>
       <c r="L7" s="1">
         <v>4</v>
@@ -1528,29 +1528,29 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" si="5"/>
-        <v>7.1337437851715861E-5</v>
+        <v>0.71337437851715868</v>
       </c>
       <c r="O7" s="1">
         <v>7</v>
       </c>
       <c r="P7" s="1">
+        <f t="shared" si="0"/>
+        <v>5607154</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="6"/>
+        <v>1.2484051624050274</v>
+      </c>
+      <c r="R7" s="1">
+        <v>7</v>
+      </c>
+      <c r="S7" s="1">
         <f t="shared" si="1"/>
         <v>5607154</v>
       </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="6"/>
-        <v>1.2484051624050274E-4</v>
-      </c>
-      <c r="R7" s="1">
-        <v>7</v>
-      </c>
-      <c r="S7" s="1">
-        <f t="shared" si="2"/>
-        <v>5607154</v>
-      </c>
       <c r="T7" s="1">
         <f t="shared" si="7"/>
-        <v>1.2484051624050274E-4</v>
+        <v>1.2484051624050274</v>
       </c>
       <c r="U7" s="1">
         <v>72</v>
@@ -1570,8 +1570,8 @@
         <v>3600188</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>8.3328981708732995E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.83328981708732985</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="4"/>
-        <v>2.7873127100065921E-5</v>
+        <v>0.2787312710006592</v>
       </c>
       <c r="L8" s="1">
         <v>4</v>
@@ -1601,29 +1601,29 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" si="5"/>
-        <v>1.1147700340896676E-4</v>
+        <v>1.1147700340896676</v>
       </c>
       <c r="O8" s="1">
         <v>1</v>
       </c>
       <c r="P8" s="1">
+        <f t="shared" si="0"/>
+        <v>3588184</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="6"/>
+        <v>0.27869250852241689</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1">
         <f t="shared" si="1"/>
         <v>3588184</v>
       </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="6"/>
-        <v>2.7869250852241689E-5</v>
-      </c>
-      <c r="R8" s="1">
-        <v>1</v>
-      </c>
-      <c r="S8" s="1">
-        <f t="shared" si="2"/>
-        <v>3588184</v>
-      </c>
       <c r="T8" s="1">
         <f t="shared" si="7"/>
-        <v>2.7869250852241689E-5</v>
+        <v>0.27869250852241689</v>
       </c>
       <c r="U8" s="1">
         <v>10</v>
@@ -1643,7 +1643,7 @@
         <v>934805</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9" s="1">
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>961939</v>
       </c>
       <c r="Q9" s="1">
@@ -1691,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>961939</v>
       </c>
       <c r="T9" s="1">
@@ -1716,8 +1716,8 @@
         <v>19897747</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>9.0462503116558874E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.90462503116558879</v>
       </c>
       <c r="F10" s="1">
         <v>38</v>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" si="3"/>
-        <v>1.8748242043949137E-4</v>
+        <v>1.8748242043949137</v>
       </c>
       <c r="I10" s="1">
         <v>29</v>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="K10" s="1">
         <f t="shared" si="4"/>
-        <v>1.4039103939183763E-4</v>
+        <v>1.4039103939183764</v>
       </c>
       <c r="L10" s="1">
         <v>32</v>
@@ -1747,29 +1747,29 @@
       </c>
       <c r="N10" s="1">
         <f t="shared" si="5"/>
-        <v>1.5249423381178399E-4</v>
+        <v>1.52494233811784</v>
       </c>
       <c r="O10" s="1">
         <v>26</v>
       </c>
       <c r="P10" s="1">
+        <f t="shared" si="0"/>
+        <v>20984400</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="6"/>
+        <v>1.239015649720745</v>
+      </c>
+      <c r="R10" s="1">
+        <v>35</v>
+      </c>
+      <c r="S10" s="1">
         <f t="shared" si="1"/>
         <v>20984400</v>
       </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="6"/>
-        <v>1.2390156497207451E-4</v>
-      </c>
-      <c r="R10" s="1">
-        <v>35</v>
-      </c>
-      <c r="S10" s="1">
-        <f t="shared" si="2"/>
-        <v>20984400</v>
-      </c>
       <c r="T10" s="1">
         <f t="shared" si="7"/>
-        <v>1.6679056823163874E-4</v>
+        <v>1.6679056823163874</v>
       </c>
       <c r="U10" s="1">
         <v>178</v>
@@ -1789,8 +1789,8 @@
         <v>10083850</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7850325024668158E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.7850325024668157</v>
       </c>
       <c r="F11" s="1">
         <v>20</v>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="3"/>
-        <v>1.9608740910000486E-4</v>
+        <v>1.9608740910000486</v>
       </c>
       <c r="I11" s="1">
         <v>16</v>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="K11" s="1">
         <f t="shared" si="4"/>
-        <v>1.5513466658651374E-4</v>
+        <v>1.5513466658651376</v>
       </c>
       <c r="L11" s="1">
         <v>17</v>
@@ -1820,29 +1820,29 @@
       </c>
       <c r="N11" s="1">
         <f t="shared" si="5"/>
-        <v>1.6300107609475118E-4</v>
+        <v>1.6300107609475116</v>
       </c>
       <c r="O11" s="1">
         <v>9</v>
       </c>
       <c r="P11" s="1">
+        <f t="shared" si="0"/>
+        <v>10429379</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="6"/>
+        <v>0.86294687344280041</v>
+      </c>
+      <c r="R11" s="1">
+        <v>15</v>
+      </c>
+      <c r="S11" s="1">
         <f t="shared" si="1"/>
         <v>10429379</v>
       </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="6"/>
-        <v>8.6294687344280041E-5</v>
-      </c>
-      <c r="R11" s="1">
-        <v>15</v>
-      </c>
-      <c r="S11" s="1">
-        <f t="shared" si="2"/>
-        <v>10429379</v>
-      </c>
       <c r="T11" s="1">
         <f t="shared" si="7"/>
-        <v>1.438244789071334E-4</v>
+        <v>1.4382447890713339</v>
       </c>
       <c r="U11" s="1">
         <v>95</v>
@@ -1862,8 +1862,8 @@
         <v>1417710</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1160886217914807E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.1160886217914809</v>
       </c>
       <c r="F12" s="1">
         <v>7</v>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="H12" s="1">
         <f t="shared" si="3"/>
-        <v>4.9077345897133881E-4</v>
+        <v>4.9077345897133888</v>
       </c>
       <c r="I12" s="1">
         <v>4</v>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="K12" s="1">
         <f t="shared" si="4"/>
-        <v>2.7997813370775739E-4</v>
+        <v>2.7997813370775742</v>
       </c>
       <c r="L12" s="1">
         <v>2</v>
@@ -1893,29 +1893,29 @@
       </c>
       <c r="N12" s="1">
         <f t="shared" si="5"/>
-        <v>1.4010134931609526E-4</v>
+        <v>1.4010134931609528</v>
       </c>
       <c r="O12" s="1">
         <v>4</v>
       </c>
       <c r="P12" s="1">
+        <f t="shared" si="0"/>
+        <v>1427538</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="6"/>
+        <v>2.8020269863219056</v>
+      </c>
+      <c r="R12" s="1">
+        <v>3</v>
+      </c>
+      <c r="S12" s="1">
         <f t="shared" si="1"/>
         <v>1427538</v>
       </c>
-      <c r="Q12" s="1">
-        <f t="shared" si="6"/>
-        <v>2.8020269863219052E-4</v>
-      </c>
-      <c r="R12" s="1">
-        <v>3</v>
-      </c>
-      <c r="S12" s="1">
-        <f t="shared" si="2"/>
-        <v>1427538</v>
-      </c>
       <c r="T12" s="1">
         <f t="shared" si="7"/>
-        <v>2.1015202397414292E-4</v>
+        <v>2.1015202397414292</v>
       </c>
       <c r="U12" s="1">
         <v>23</v>
@@ -1935,8 +1935,8 @@
         <v>1630391</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>1.8400494114601958E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.8400494114601957</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="3"/>
-        <v>6.0630900902430328E-5</v>
+        <v>0.60630900902430329</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -1966,29 +1966,29 @@
       </c>
       <c r="N13" s="1">
         <f t="shared" si="5"/>
-        <v>5.8243051749533916E-5</v>
+        <v>0.58243051749533914</v>
       </c>
       <c r="O13" s="1">
         <v>2</v>
       </c>
       <c r="P13" s="1">
+        <f t="shared" si="0"/>
+        <v>1716943</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="6"/>
+        <v>1.1648610349906783</v>
+      </c>
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1">
         <f t="shared" si="1"/>
         <v>1716943</v>
       </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1648610349906783E-4</v>
-      </c>
-      <c r="R13" s="1">
-        <v>1</v>
-      </c>
-      <c r="S13" s="1">
-        <f t="shared" si="2"/>
-        <v>1716943</v>
-      </c>
       <c r="T13" s="1">
         <f t="shared" si="7"/>
-        <v>5.8243051749533916E-5</v>
+        <v>0.58243051749533914</v>
       </c>
       <c r="U13" s="1">
         <v>8</v>
@@ -2008,8 +2008,8 @@
         <v>12882438</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>8.5387564062019939E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.85387564062019938</v>
       </c>
       <c r="F14" s="1">
         <v>16</v>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="3"/>
-        <v>1.2439695659735759E-4</v>
+        <v>1.2439695659735759</v>
       </c>
       <c r="I14" s="1">
         <v>4</v>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="K14" s="1">
         <f t="shared" si="4"/>
-        <v>3.1163021086614035E-5</v>
+        <v>0.31163021086614034</v>
       </c>
       <c r="L14" s="1">
         <v>11</v>
@@ -2039,29 +2039,29 @@
       </c>
       <c r="N14" s="1">
         <f t="shared" si="5"/>
-        <v>8.5923919992957369E-5</v>
+        <v>0.85923919992957365</v>
       </c>
       <c r="O14" s="1">
         <v>12</v>
       </c>
       <c r="P14" s="1">
+        <f t="shared" si="0"/>
+        <v>12802023</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.93735185446862579</v>
+      </c>
+      <c r="R14" s="1">
+        <v>8</v>
+      </c>
+      <c r="S14" s="1">
         <f t="shared" si="1"/>
         <v>12802023</v>
       </c>
-      <c r="Q14" s="1">
-        <f t="shared" si="6"/>
-        <v>9.3735185446862574E-5</v>
-      </c>
-      <c r="R14" s="1">
-        <v>8</v>
-      </c>
-      <c r="S14" s="1">
-        <f t="shared" si="2"/>
-        <v>12802023</v>
-      </c>
       <c r="T14" s="1">
         <f t="shared" si="7"/>
-        <v>6.2490123631241712E-5</v>
+        <v>0.62490123631241712</v>
       </c>
       <c r="U14" s="1">
         <v>62</v>
@@ -2081,8 +2081,8 @@
         <v>6593182</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>7.5835916557437662E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.75835916557437666</v>
       </c>
       <c r="F15" s="1">
         <v>8</v>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="3"/>
-        <v>1.2101783258272024E-4</v>
+        <v>1.2101783258272023</v>
       </c>
       <c r="I15" s="1">
         <v>3</v>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="K15" s="1">
         <f t="shared" si="4"/>
-        <v>4.5221538053848905E-5</v>
+        <v>0.45221538053848903</v>
       </c>
       <c r="L15" s="1">
         <v>7</v>
@@ -2112,29 +2112,29 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" si="5"/>
-        <v>1.0499761655410422E-4</v>
+        <v>1.0499761655410422</v>
       </c>
       <c r="O15" s="1">
         <v>3</v>
       </c>
       <c r="P15" s="1">
+        <f t="shared" si="0"/>
+        <v>6666818</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="6"/>
+        <v>0.44998978523187527</v>
+      </c>
+      <c r="R15" s="1">
+        <v>9</v>
+      </c>
+      <c r="S15" s="1">
         <f t="shared" si="1"/>
         <v>6666818</v>
       </c>
-      <c r="Q15" s="1">
-        <f t="shared" si="6"/>
-        <v>4.4998978523187525E-5</v>
-      </c>
-      <c r="R15" s="1">
-        <v>9</v>
-      </c>
-      <c r="S15" s="1">
-        <f t="shared" si="2"/>
-        <v>6666818</v>
-      </c>
       <c r="T15" s="1">
         <f t="shared" si="7"/>
-        <v>1.3499693556956257E-4</v>
+        <v>1.3499693556956256</v>
       </c>
       <c r="U15" s="1">
         <v>35</v>
@@ -2154,8 +2154,8 @@
         <v>3105563</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>6.4400561186490175E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.64400561186490179</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" si="3"/>
-        <v>3.2066976369524443E-5</v>
+        <v>0.32066976369524447</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
@@ -2185,29 +2185,29 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="5"/>
-        <v>3.1789315674580405E-5</v>
+        <v>0.31789315674580404</v>
       </c>
       <c r="O16" s="1">
         <v>1</v>
       </c>
       <c r="P16" s="1">
+        <f t="shared" si="0"/>
+        <v>3145711</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="6"/>
+        <v>0.31789315674580404</v>
+      </c>
+      <c r="R16" s="1">
+        <v>1</v>
+      </c>
+      <c r="S16" s="1">
         <f t="shared" si="1"/>
         <v>3145711</v>
       </c>
-      <c r="Q16" s="1">
-        <f t="shared" si="6"/>
-        <v>3.1789315674580405E-5</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1</v>
-      </c>
-      <c r="S16" s="1">
-        <f t="shared" si="2"/>
-        <v>3145711</v>
-      </c>
       <c r="T16" s="1">
         <f t="shared" si="7"/>
-        <v>3.1789315674580405E-5</v>
+        <v>0.31789315674580404</v>
       </c>
       <c r="U16" s="1">
         <v>6</v>
@@ -2227,8 +2227,8 @@
         <v>2899553</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>1.3795229816457915E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.3795229816457917</v>
       </c>
       <c r="F17" s="1">
         <v>7</v>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="H17" s="1">
         <f t="shared" si="3"/>
-        <v>2.4089842724299665E-4</v>
+        <v>2.4089842724299664</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="K17" s="1">
         <f t="shared" si="4"/>
-        <v>3.439107675366119E-5</v>
+        <v>0.34391076753661187</v>
       </c>
       <c r="L17" s="1">
         <v>3</v>
@@ -2258,29 +2258,29 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" si="5"/>
-        <v>1.0298226336478069E-4</v>
+        <v>1.0298226336478069</v>
       </c>
       <c r="O17" s="1">
         <v>5</v>
       </c>
       <c r="P17" s="1">
+        <f t="shared" si="0"/>
+        <v>2913123</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="6"/>
+        <v>1.7163710560796781</v>
+      </c>
+      <c r="R17" s="1">
+        <v>2</v>
+      </c>
+      <c r="S17" s="1">
         <f t="shared" si="1"/>
         <v>2913123</v>
       </c>
-      <c r="Q17" s="1">
-        <f t="shared" si="6"/>
-        <v>1.716371056079678E-4</v>
-      </c>
-      <c r="R17" s="1">
-        <v>2</v>
-      </c>
-      <c r="S17" s="1">
-        <f t="shared" si="2"/>
-        <v>2913123</v>
-      </c>
       <c r="T17" s="1">
         <f t="shared" si="7"/>
-        <v>6.8654842243187124E-5</v>
+        <v>0.6865484224318712</v>
       </c>
       <c r="U17" s="1">
         <v>22</v>
@@ -2300,8 +2300,8 @@
         <v>4410415</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
-        <v>4.534720655539218E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.45347206555392178</v>
       </c>
       <c r="F18" s="1">
         <v>5</v>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" si="3"/>
-        <v>1.1306955111614347E-4</v>
+        <v>1.1306955111614347</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="K18" s="1">
         <f t="shared" si="4"/>
-        <v>2.254225715170015E-5</v>
+        <v>0.22542257151700149</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
@@ -2337,18 +2337,18 @@
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4454189</v>
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="6"/>
-        <v>2.2450776112104807E-5</v>
+        <v>0.22450776112104806</v>
       </c>
       <c r="R18" s="1">
         <v>0</v>
       </c>
       <c r="S18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4454189</v>
       </c>
       <c r="T18" s="1">
@@ -2373,8 +2373,8 @@
         <v>4648797</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5057659002963564E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.5057659002963564</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" si="3"/>
-        <v>4.2815449783792679E-5</v>
+        <v>0.42815449783792681</v>
       </c>
       <c r="I19" s="1">
         <v>2</v>
@@ -2394,7 +2394,7 @@
       </c>
       <c r="K19" s="1">
         <f t="shared" si="4"/>
-        <v>4.2678894454453829E-5</v>
+        <v>0.42678894454453831</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
@@ -2404,29 +2404,29 @@
       </c>
       <c r="N19" s="1">
         <f t="shared" si="5"/>
-        <v>2.134775644686234E-5</v>
+        <v>0.2134775644686234</v>
       </c>
       <c r="O19" s="1">
         <v>0</v>
       </c>
       <c r="P19" s="1">
+        <f t="shared" si="0"/>
+        <v>4684333</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>5</v>
+      </c>
+      <c r="S19" s="1">
         <f t="shared" si="1"/>
         <v>4684333</v>
       </c>
-      <c r="Q19" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="1">
-        <v>5</v>
-      </c>
-      <c r="S19" s="1">
-        <f t="shared" si="2"/>
-        <v>4684333</v>
-      </c>
       <c r="T19" s="1">
         <f t="shared" si="7"/>
-        <v>1.067387822343117E-4</v>
+        <v>1.067387822343117</v>
       </c>
       <c r="U19" s="1">
         <v>17</v>
@@ -2446,8 +2446,8 @@
         <v>1328903</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
-        <v>7.525003706064325E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.7525003706064326</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" si="3"/>
-        <v>7.5313284434928195E-5</v>
+        <v>0.75313284434928196</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="K20" s="1">
         <f t="shared" si="4"/>
-        <v>7.5174856716723099E-5</v>
+        <v>0.75174856716723104</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -2483,23 +2483,23 @@
         <v>0</v>
       </c>
       <c r="P20" s="1">
+        <f t="shared" si="0"/>
+        <v>1335907</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1">
         <f t="shared" si="1"/>
         <v>1335907</v>
       </c>
-      <c r="Q20" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="1">
-        <v>1</v>
-      </c>
-      <c r="S20" s="1">
-        <f t="shared" si="2"/>
-        <v>1335907</v>
-      </c>
       <c r="T20" s="1">
         <f t="shared" si="7"/>
-        <v>7.4855510151530016E-5</v>
+        <v>0.74855510151530014</v>
       </c>
       <c r="U20" s="1">
         <v>4</v>
@@ -2519,8 +2519,8 @@
         <v>5970245</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
-        <v>3.3499462752366108E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.3349946275236611</v>
       </c>
       <c r="F21" s="1">
         <v>5</v>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" si="3"/>
-        <v>8.3325542395119384E-5</v>
+        <v>0.8332554239511939</v>
       </c>
       <c r="I21" s="1">
         <v>4</v>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="K21" s="1">
         <f t="shared" si="4"/>
-        <v>6.6392774341582849E-5</v>
+        <v>0.6639277434158285</v>
       </c>
       <c r="L21" s="1">
         <v>4</v>
@@ -2550,29 +2550,29 @@
       </c>
       <c r="N21" s="1">
         <f t="shared" si="5"/>
-        <v>6.6091920312310763E-5</v>
+        <v>0.6609192031231077</v>
       </c>
       <c r="O21" s="1">
         <v>7</v>
       </c>
       <c r="P21" s="1">
+        <f t="shared" si="0"/>
+        <v>6052177</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="6"/>
+        <v>1.1566086054654383</v>
+      </c>
+      <c r="R21" s="1">
+        <v>4</v>
+      </c>
+      <c r="S21" s="1">
         <f t="shared" si="1"/>
         <v>6052177</v>
       </c>
-      <c r="Q21" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1566086054654383E-4</v>
-      </c>
-      <c r="R21" s="1">
-        <v>4</v>
-      </c>
-      <c r="S21" s="1">
-        <f t="shared" si="2"/>
-        <v>6052177</v>
-      </c>
       <c r="T21" s="1">
         <f t="shared" si="7"/>
-        <v>6.6091920312310763E-5</v>
+        <v>0.6609192031231077</v>
       </c>
       <c r="U21" s="1">
         <v>26</v>
@@ -2592,8 +2592,8 @@
         <v>6757925</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>7.398720761180391E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.73987207611803918</v>
       </c>
       <c r="F22" s="1">
         <v>9</v>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="3"/>
-        <v>1.3246978732122834E-4</v>
+        <v>1.3246978732122834</v>
       </c>
       <c r="I22" s="1">
         <v>4</v>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="K22" s="1">
         <f t="shared" si="4"/>
-        <v>5.861904377391749E-5</v>
+        <v>0.5861904377391749</v>
       </c>
       <c r="L22" s="1">
         <v>4</v>
@@ -2623,29 +2623,29 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" si="5"/>
-        <v>5.8310576416083283E-5</v>
+        <v>0.58310576416083282</v>
       </c>
       <c r="O22" s="1">
         <v>4</v>
       </c>
       <c r="P22" s="1">
+        <f t="shared" si="0"/>
+        <v>6859819</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="6"/>
+        <v>0.58310576416083282</v>
+      </c>
+      <c r="R22" s="1">
+        <v>8</v>
+      </c>
+      <c r="S22" s="1">
         <f t="shared" si="1"/>
         <v>6859819</v>
       </c>
-      <c r="Q22" s="1">
-        <f t="shared" si="6"/>
-        <v>5.8310576416083283E-5</v>
-      </c>
-      <c r="R22" s="1">
-        <v>8</v>
-      </c>
-      <c r="S22" s="1">
-        <f t="shared" si="2"/>
-        <v>6859819</v>
-      </c>
       <c r="T22" s="1">
         <f t="shared" si="7"/>
-        <v>1.1662115283216657E-4</v>
+        <v>1.1662115283216656</v>
       </c>
       <c r="U22" s="1">
         <v>34</v>
@@ -2665,8 +2665,8 @@
         <v>9914675</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>5.0430296504928293E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.50430296504928296</v>
       </c>
       <c r="F23" s="1">
         <v>4</v>
@@ -2676,7 +2676,7 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" si="3"/>
-        <v>4.033002055822798E-5</v>
+        <v>0.4033002055822798</v>
       </c>
       <c r="I23" s="1">
         <v>5</v>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="K23" s="1">
         <f t="shared" si="4"/>
-        <v>5.0335004623270176E-5</v>
+        <v>0.50335004623270174</v>
       </c>
       <c r="L23" s="1">
         <v>10</v>
@@ -2696,29 +2696,29 @@
       </c>
       <c r="N23" s="1">
         <f t="shared" si="5"/>
-        <v>1.0037831583454884E-4</v>
+        <v>1.0037831583454884</v>
       </c>
       <c r="O23" s="1">
         <v>8</v>
       </c>
       <c r="P23" s="1">
+        <f t="shared" si="0"/>
+        <v>9962311</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="6"/>
+        <v>0.80302652667639063</v>
+      </c>
+      <c r="R23" s="1">
+        <v>16</v>
+      </c>
+      <c r="S23" s="1">
         <f t="shared" si="1"/>
         <v>9962311</v>
       </c>
-      <c r="Q23" s="1">
-        <f t="shared" si="6"/>
-        <v>8.0302652667639055E-5</v>
-      </c>
-      <c r="R23" s="1">
-        <v>16</v>
-      </c>
-      <c r="S23" s="1">
-        <f t="shared" si="2"/>
-        <v>9962311</v>
-      </c>
       <c r="T23" s="1">
         <f t="shared" si="7"/>
-        <v>1.6060530533527811E-4</v>
+        <v>1.6060530533527813</v>
       </c>
       <c r="U23" s="1">
         <v>48</v>
@@ -2738,8 +2738,8 @@
         <v>5452649</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
-        <v>5.5019129234249261E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.55019129234249264</v>
       </c>
       <c r="F24" s="1">
         <v>5</v>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" si="3"/>
-        <v>9.1186995713116956E-5</v>
+        <v>0.91186995713116958</v>
       </c>
       <c r="I24" s="1">
         <v>7</v>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="K24" s="1">
         <f t="shared" si="4"/>
-        <v>1.266956860118913E-4</v>
+        <v>1.266956860118913</v>
       </c>
       <c r="L24" s="1">
         <v>6</v>
@@ -2769,29 +2769,29 @@
       </c>
       <c r="N24" s="1">
         <f t="shared" si="5"/>
-        <v>1.0759232407668751E-4</v>
+        <v>1.0759232407668751</v>
       </c>
       <c r="O24" s="1">
         <v>4</v>
       </c>
       <c r="P24" s="1">
+        <f t="shared" si="0"/>
+        <v>5576606</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="6"/>
+        <v>0.71728216051125004</v>
+      </c>
+      <c r="R24" s="1">
+        <v>4</v>
+      </c>
+      <c r="S24" s="1">
         <f t="shared" si="1"/>
         <v>5576606</v>
       </c>
-      <c r="Q24" s="1">
-        <f t="shared" si="6"/>
-        <v>7.1728216051125004E-5</v>
-      </c>
-      <c r="R24" s="1">
-        <v>4</v>
-      </c>
-      <c r="S24" s="1">
-        <f t="shared" si="2"/>
-        <v>5576606</v>
-      </c>
       <c r="T24" s="1">
         <f t="shared" si="7"/>
-        <v>7.1728216051125004E-5</v>
+        <v>0.71728216051125004</v>
       </c>
       <c r="U24" s="1">
         <v>29</v>
@@ -2811,7 +2811,7 @@
         <v>2988578</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F25" s="1">
@@ -2848,23 +2848,23 @@
         <v>3</v>
       </c>
       <c r="P25" s="1">
+        <f t="shared" si="0"/>
+        <v>2984100</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="6"/>
+        <v>1.0053282396702523</v>
+      </c>
+      <c r="R25" s="1">
+        <v>1</v>
+      </c>
+      <c r="S25" s="1">
         <f t="shared" si="1"/>
         <v>2984100</v>
       </c>
-      <c r="Q25" s="1">
-        <f t="shared" si="6"/>
-        <v>1.0053282396702523E-4</v>
-      </c>
-      <c r="R25" s="1">
-        <v>1</v>
-      </c>
-      <c r="S25" s="1">
-        <f t="shared" si="2"/>
-        <v>2984100</v>
-      </c>
       <c r="T25" s="1">
         <f t="shared" si="7"/>
-        <v>3.3510941322341746E-5</v>
+        <v>0.33510941322341747</v>
       </c>
       <c r="U25" s="1">
         <v>4</v>
@@ -2884,8 +2884,8 @@
         <v>6058014</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6507059904450534E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.6507059904450534</v>
       </c>
       <c r="F26" s="1">
         <v>18</v>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="H26" s="1">
         <f t="shared" si="3"/>
-        <v>2.9641144543394635E-4</v>
+        <v>2.9641144543394637</v>
       </c>
       <c r="I26" s="1">
         <v>7</v>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="K26" s="1">
         <f t="shared" si="4"/>
-        <v>1.1492033722223755E-4</v>
+        <v>1.1492033722223756</v>
       </c>
       <c r="L26" s="1">
         <v>10</v>
@@ -2915,29 +2915,29 @@
       </c>
       <c r="N26" s="1">
         <f t="shared" si="5"/>
-        <v>1.6357156550419626E-4</v>
+        <v>1.6357156550419627</v>
       </c>
       <c r="O26" s="1">
         <v>10</v>
       </c>
       <c r="P26" s="1">
+        <f t="shared" si="0"/>
+        <v>6113532</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="6"/>
+        <v>1.6357156550419627</v>
+      </c>
+      <c r="R26" s="1">
+        <v>7</v>
+      </c>
+      <c r="S26" s="1">
         <f t="shared" si="1"/>
         <v>6113532</v>
       </c>
-      <c r="Q26" s="1">
-        <f t="shared" si="6"/>
-        <v>1.6357156550419626E-4</v>
-      </c>
-      <c r="R26" s="1">
-        <v>7</v>
-      </c>
-      <c r="S26" s="1">
-        <f t="shared" si="2"/>
-        <v>6113532</v>
-      </c>
       <c r="T26" s="1">
         <f t="shared" si="7"/>
-        <v>1.145000958529374E-4</v>
+        <v>1.1450009585293739</v>
       </c>
       <c r="U26" s="1">
         <v>62</v>
@@ -2957,8 +2957,8 @@
         <v>1019931</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
-        <v>7.843667855962804E-4</v>
+        <f t="shared" si="2"/>
+        <v>7.8436678559628046</v>
       </c>
       <c r="F27" s="1">
         <v>5</v>
@@ -2968,7 +2968,7 @@
       </c>
       <c r="H27" s="1">
         <f t="shared" si="3"/>
-        <v>4.8623138584697129E-4</v>
+        <v>4.8623138584697125</v>
       </c>
       <c r="I27" s="1">
         <v>2</v>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="K27" s="1">
         <f t="shared" si="4"/>
-        <v>1.9255653459855816E-4</v>
+        <v>1.9255653459855815</v>
       </c>
       <c r="L27" s="1">
         <v>4</v>
@@ -2988,29 +2988,29 @@
       </c>
       <c r="N27" s="1">
         <f t="shared" si="5"/>
-        <v>3.8077359868176177E-4</v>
+        <v>3.8077359868176179</v>
       </c>
       <c r="O27" s="1">
         <v>1</v>
       </c>
       <c r="P27" s="1">
+        <f t="shared" si="0"/>
+        <v>1050493</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="6"/>
+        <v>0.95193399670440448</v>
+      </c>
+      <c r="R27" s="1">
+        <v>1</v>
+      </c>
+      <c r="S27" s="1">
         <f t="shared" si="1"/>
         <v>1050493</v>
       </c>
-      <c r="Q27" s="1">
-        <f t="shared" si="6"/>
-        <v>9.5193399670440442E-5</v>
-      </c>
-      <c r="R27" s="1">
-        <v>1</v>
-      </c>
-      <c r="S27" s="1">
-        <f t="shared" si="2"/>
-        <v>1050493</v>
-      </c>
       <c r="T27" s="1">
         <f t="shared" si="7"/>
-        <v>9.5193399670440442E-5</v>
+        <v>0.95193399670440448</v>
       </c>
       <c r="U27" s="1">
         <v>21</v>
@@ -3030,8 +3030,8 @@
         <v>1880920</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1266188886289689E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.1266188886289692</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -3067,23 +3067,23 @@
         <v>3</v>
       </c>
       <c r="P28" s="1">
+        <f t="shared" si="0"/>
+        <v>1920076</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="6"/>
+        <v>1.5624381534897578</v>
+      </c>
+      <c r="R28" s="1">
+        <v>3</v>
+      </c>
+      <c r="S28" s="1">
         <f t="shared" si="1"/>
         <v>1920076</v>
       </c>
-      <c r="Q28" s="1">
-        <f t="shared" si="6"/>
-        <v>1.5624381534897578E-4</v>
-      </c>
-      <c r="R28" s="1">
-        <v>3</v>
-      </c>
-      <c r="S28" s="1">
-        <f t="shared" si="2"/>
-        <v>1920076</v>
-      </c>
       <c r="T28" s="1">
         <f t="shared" si="7"/>
-        <v>1.5624381534897578E-4</v>
+        <v>1.5624381534897578</v>
       </c>
       <c r="U28" s="1">
         <v>10</v>
@@ -3103,8 +3103,8 @@
         <v>2831730</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
-        <v>2.1188460764267779E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.1188460764267778</v>
       </c>
       <c r="F29" s="1">
         <v>7</v>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="H29" s="1">
         <f t="shared" si="3"/>
-        <v>2.4279783576946275E-4</v>
+        <v>2.4279783576946277</v>
       </c>
       <c r="I29" s="1">
         <v>7</v>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="K29" s="1">
         <f t="shared" si="4"/>
-        <v>2.3815566807087782E-4</v>
+        <v>2.3815566807087785</v>
       </c>
       <c r="L29" s="1">
         <v>3</v>
@@ -3134,29 +3134,29 @@
       </c>
       <c r="N29" s="1">
         <f t="shared" si="5"/>
-        <v>1.0006540942262591E-4</v>
+        <v>1.0006540942262592</v>
       </c>
       <c r="O29" s="1">
         <v>2</v>
       </c>
       <c r="P29" s="1">
+        <f t="shared" si="0"/>
+        <v>2998039</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="6"/>
+        <v>0.66710272948417282</v>
+      </c>
+      <c r="R29" s="1">
+        <v>1</v>
+      </c>
+      <c r="S29" s="1">
         <f t="shared" si="1"/>
         <v>2998039</v>
       </c>
-      <c r="Q29" s="1">
-        <f t="shared" si="6"/>
-        <v>6.6710272948417276E-5</v>
-      </c>
-      <c r="R29" s="1">
-        <v>1</v>
-      </c>
-      <c r="S29" s="1">
-        <f t="shared" si="2"/>
-        <v>2998039</v>
-      </c>
       <c r="T29" s="1">
         <f t="shared" si="7"/>
-        <v>3.3355136474208638E-5</v>
+        <v>0.33355136474208641</v>
       </c>
       <c r="U29" s="1">
         <v>26</v>
@@ -3176,8 +3176,8 @@
         <v>1328684</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
-        <v>3.763122006436444E-4</v>
+        <f t="shared" si="2"/>
+        <v>3.7631220064364439</v>
       </c>
       <c r="F30" s="1">
         <v>3</v>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="H30" s="1">
         <f t="shared" si="3"/>
-        <v>2.2554118607598933E-4</v>
+        <v>2.2554118607598936</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="K30" s="1">
         <f t="shared" si="4"/>
-        <v>7.4905525406081572E-5</v>
+        <v>0.74905525406081575</v>
       </c>
       <c r="L30" s="1">
         <v>1</v>
@@ -3207,24 +3207,24 @@
       </c>
       <c r="N30" s="1">
         <f t="shared" si="5"/>
-        <v>7.4471531395335842E-5</v>
+        <v>0.74471531395335844</v>
       </c>
       <c r="O30" s="1">
         <v>1</v>
       </c>
       <c r="P30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1342795</v>
       </c>
       <c r="Q30" s="1">
         <f t="shared" si="6"/>
-        <v>7.4471531395335842E-5</v>
+        <v>0.74471531395335844</v>
       </c>
       <c r="R30" s="1">
         <v>0</v>
       </c>
       <c r="S30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1342795</v>
       </c>
       <c r="T30" s="1">
@@ -3249,8 +3249,8 @@
         <v>8943010</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2363834995152637E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.22363834995152637</v>
       </c>
       <c r="F31" s="1">
         <v>6</v>
@@ -3260,7 +3260,7 @@
       </c>
       <c r="H31" s="1">
         <f t="shared" si="3"/>
-        <v>6.696427824059394E-5</v>
+        <v>0.66964278240593944</v>
       </c>
       <c r="I31" s="1">
         <v>8</v>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="K31" s="1">
         <f t="shared" si="4"/>
-        <v>8.9102576668312089E-5</v>
+        <v>0.89102576668312095</v>
       </c>
       <c r="L31" s="1">
         <v>2</v>
@@ -3280,29 +3280,29 @@
       </c>
       <c r="N31" s="1">
         <f t="shared" si="5"/>
-        <v>2.2208295153572581E-5</v>
+        <v>0.22208295153572583</v>
       </c>
       <c r="O31" s="1">
         <v>2</v>
       </c>
       <c r="P31" s="1">
+        <f t="shared" si="0"/>
+        <v>9005644</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="6"/>
+        <v>0.22208295153572583</v>
+      </c>
+      <c r="R31" s="1">
+        <v>3</v>
+      </c>
+      <c r="S31" s="1">
         <f t="shared" si="1"/>
         <v>9005644</v>
       </c>
-      <c r="Q31" s="1">
-        <f t="shared" si="6"/>
-        <v>2.2208295153572581E-5</v>
-      </c>
-      <c r="R31" s="1">
-        <v>3</v>
-      </c>
-      <c r="S31" s="1">
-        <f t="shared" si="2"/>
-        <v>9005644</v>
-      </c>
       <c r="T31" s="1">
         <f t="shared" si="7"/>
-        <v>3.3312442730358873E-5</v>
+        <v>0.33312442730358871</v>
       </c>
       <c r="U31" s="1">
         <v>23</v>
@@ -3322,8 +3322,8 @@
         <v>2083207</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
-        <v>9.6005821793033539E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.9600582179303353</v>
       </c>
       <c r="F32" s="1">
         <v>2</v>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" si="3"/>
-        <v>9.6049300184798854E-5</v>
+        <v>0.96049300184798847</v>
       </c>
       <c r="I32" s="1">
         <v>1</v>
@@ -3343,7 +3343,7 @@
       </c>
       <c r="K32" s="1">
         <f t="shared" si="4"/>
-        <v>4.7951695380141865E-5</v>
+        <v>0.47951695380141862</v>
       </c>
       <c r="L32" s="1">
         <v>1</v>
@@ -3353,29 +3353,29 @@
       </c>
       <c r="N32" s="1">
         <f t="shared" si="5"/>
-        <v>4.7891114761478308E-5</v>
+        <v>0.47891114761478304</v>
       </c>
       <c r="O32" s="1">
         <v>4</v>
       </c>
       <c r="P32" s="1">
+        <f t="shared" si="0"/>
+        <v>2088070</v>
+      </c>
+      <c r="Q32" s="1">
+        <f t="shared" si="6"/>
+        <v>1.9156445904591322</v>
+      </c>
+      <c r="R32" s="1">
+        <v>6</v>
+      </c>
+      <c r="S32" s="1">
         <f t="shared" si="1"/>
         <v>2088070</v>
       </c>
-      <c r="Q32" s="1">
-        <f t="shared" si="6"/>
-        <v>1.9156445904591323E-4</v>
-      </c>
-      <c r="R32" s="1">
-        <v>6</v>
-      </c>
-      <c r="S32" s="1">
-        <f t="shared" si="2"/>
-        <v>2088070</v>
-      </c>
       <c r="T32" s="1">
         <f t="shared" si="7"/>
-        <v>2.8734668856886979E-4</v>
+        <v>2.873466885688698</v>
       </c>
       <c r="U32" s="1">
         <v>16</v>
@@ -3395,8 +3395,8 @@
         <v>19773580</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
-        <v>6.5744291119766869E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.65744291119766873</v>
       </c>
       <c r="F33" s="1">
         <v>18</v>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="H33" s="1">
         <f t="shared" si="3"/>
-        <v>9.0820348420157337E-5</v>
+        <v>0.90820348420157337</v>
       </c>
       <c r="I33" s="1">
         <v>12</v>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="K33" s="1">
         <f t="shared" si="4"/>
-        <v>6.0495195521984307E-5</v>
+        <v>0.60495195521984313</v>
       </c>
       <c r="L33" s="1">
         <v>9</v>
@@ -3426,29 +3426,29 @@
       </c>
       <c r="N33" s="1">
         <f t="shared" si="5"/>
-        <v>4.5341423183643996E-5</v>
+        <v>0.45341423183643997</v>
       </c>
       <c r="O33" s="1">
         <v>9</v>
       </c>
       <c r="P33" s="1">
+        <f t="shared" si="0"/>
+        <v>19849399</v>
+      </c>
+      <c r="Q33" s="1">
+        <f t="shared" si="6"/>
+        <v>0.45341423183643997</v>
+      </c>
+      <c r="R33" s="1">
+        <v>14</v>
+      </c>
+      <c r="S33" s="1">
         <f t="shared" si="1"/>
         <v>19849399</v>
       </c>
-      <c r="Q33" s="1">
-        <f t="shared" si="6"/>
-        <v>4.5341423183643996E-5</v>
-      </c>
-      <c r="R33" s="1">
-        <v>14</v>
-      </c>
-      <c r="S33" s="1">
-        <f t="shared" si="2"/>
-        <v>19849399</v>
-      </c>
       <c r="T33" s="1">
-        <f>(R33/S33)*100</f>
-        <v>7.0531102730112888E-5</v>
+        <f t="shared" si="7"/>
+        <v>0.70531102730112882</v>
       </c>
       <c r="U33" s="1">
         <v>75</v>
@@ -3468,8 +3468,8 @@
         <v>9941160</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" ref="E34:E51" si="8">(C34/D34)*100</f>
-        <v>1.005918826374387E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.005918826374387</v>
       </c>
       <c r="F34" s="1">
         <v>7</v>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H34" s="1">
         <f t="shared" si="3"/>
-        <v>6.9708833174712535E-5</v>
+        <v>0.69708833174712537</v>
       </c>
       <c r="I34" s="1">
         <v>16</v>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="K34" s="1">
         <f t="shared" si="4"/>
-        <v>1.5753165229338026E-4</v>
+        <v>1.5753165229338026</v>
       </c>
       <c r="L34" s="1">
         <v>32</v>
@@ -3499,29 +3499,29 @@
       </c>
       <c r="N34" s="1">
         <f t="shared" si="5"/>
-        <v>3.1148345064092099E-4</v>
+        <v>3.1148345064092098</v>
       </c>
       <c r="O34" s="1">
         <v>14</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" ref="P34:P51" si="9">M34</f>
+        <f t="shared" ref="P34:P51" si="8">M34</f>
         <v>10273419</v>
       </c>
       <c r="Q34" s="1">
         <f t="shared" si="6"/>
-        <v>1.3627400965540292E-4</v>
+        <v>1.3627400965540293</v>
       </c>
       <c r="R34" s="1">
         <v>20</v>
       </c>
       <c r="S34" s="1">
-        <f t="shared" ref="S34:S51" si="10">M34</f>
+        <f t="shared" ref="S34:S51" si="9">M34</f>
         <v>10273419</v>
       </c>
       <c r="T34" s="1">
         <f t="shared" si="7"/>
-        <v>1.9467715665057563E-4</v>
+        <v>1.9467715665057563</v>
       </c>
       <c r="U34" s="1">
         <v>99</v>
@@ -3541,7 +3541,7 @@
         <v>738658</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F35" s="1">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" si="3"/>
-        <v>1.3247507150341984E-4</v>
+        <v>1.3247507150341984</v>
       </c>
       <c r="I35" s="1">
         <v>1</v>
@@ -3562,7 +3562,7 @@
       </c>
       <c r="K35" s="1">
         <f t="shared" si="4"/>
-        <v>1.3235426471911777E-4</v>
+        <v>1.3235426471911778</v>
       </c>
       <c r="L35" s="1">
         <v>0</v>
@@ -3578,7 +3578,7 @@
         <v>0</v>
       </c>
       <c r="P35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>755393</v>
       </c>
       <c r="Q35" s="1">
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="S35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>755393</v>
       </c>
       <c r="T35" s="1">
@@ -3614,8 +3614,8 @@
         <v>11593741</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="8"/>
-        <v>9.4878779851990827E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.94878779851990835</v>
       </c>
       <c r="F36" s="1">
         <v>7</v>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="H36" s="1">
         <f t="shared" si="3"/>
-        <v>6.0313490568305593E-5</v>
+        <v>0.60313490568305594</v>
       </c>
       <c r="I36" s="1">
         <v>9</v>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="K36" s="1">
         <f t="shared" si="4"/>
-        <v>7.7435647965154642E-5</v>
+        <v>0.77435647965154653</v>
       </c>
       <c r="L36" s="1">
         <v>11</v>
@@ -3645,29 +3645,29 @@
       </c>
       <c r="N36" s="1">
         <f t="shared" si="5"/>
-        <v>9.4350878393811819E-5</v>
+        <v>0.9435087839381181</v>
       </c>
       <c r="O36" s="1">
         <v>11</v>
       </c>
       <c r="P36" s="1">
+        <f t="shared" si="8"/>
+        <v>11658609</v>
+      </c>
+      <c r="Q36" s="1">
+        <f t="shared" si="6"/>
+        <v>0.9435087839381181</v>
+      </c>
+      <c r="R36" s="1">
+        <v>10</v>
+      </c>
+      <c r="S36" s="1">
         <f t="shared" si="9"/>
         <v>11658609</v>
       </c>
-      <c r="Q36" s="1">
-        <f t="shared" si="6"/>
-        <v>9.4350878393811819E-5</v>
-      </c>
-      <c r="R36" s="1">
-        <v>10</v>
-      </c>
-      <c r="S36" s="1">
-        <f t="shared" si="10"/>
-        <v>11658609</v>
-      </c>
       <c r="T36" s="1">
         <f t="shared" si="7"/>
-        <v>8.5773525812556195E-5</v>
+        <v>0.85773525812556195</v>
       </c>
       <c r="U36" s="1">
         <v>59</v>
@@ -3687,8 +3687,8 @@
         <v>3875008</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="8"/>
-        <v>2.5806398335177631E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.25806398335177627</v>
       </c>
       <c r="F37" s="1">
         <v>2</v>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="H37" s="1">
         <f t="shared" si="3"/>
-        <v>5.1224876439194917E-5</v>
+        <v>0.51224876439194911</v>
       </c>
       <c r="I37" s="1">
         <v>0</v>
@@ -3718,29 +3718,29 @@
       </c>
       <c r="N37" s="1">
         <f t="shared" si="5"/>
-        <v>2.5439699770839183E-5</v>
+        <v>0.2543969977083918</v>
       </c>
       <c r="O37" s="1">
         <v>2</v>
       </c>
       <c r="P37" s="1">
+        <f t="shared" si="8"/>
+        <v>3930864</v>
+      </c>
+      <c r="Q37" s="1">
+        <f t="shared" si="6"/>
+        <v>0.50879399541678361</v>
+      </c>
+      <c r="R37" s="1">
+        <v>4</v>
+      </c>
+      <c r="S37" s="1">
         <f t="shared" si="9"/>
         <v>3930864</v>
       </c>
-      <c r="Q37" s="1">
-        <f t="shared" si="6"/>
-        <v>5.0879399541678366E-5</v>
-      </c>
-      <c r="R37" s="1">
-        <v>4</v>
-      </c>
-      <c r="S37" s="1">
-        <f t="shared" si="10"/>
-        <v>3930864</v>
-      </c>
       <c r="T37" s="1">
         <f t="shared" si="7"/>
-        <v>1.0175879908335673E-4</v>
+        <v>1.0175879908335672</v>
       </c>
       <c r="U37" s="1">
         <v>10</v>
@@ -3760,8 +3760,8 @@
         <v>3960673</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="8"/>
-        <v>3.5347528058994013E-4</v>
+        <f t="shared" si="2"/>
+        <v>3.5347528058994016</v>
       </c>
       <c r="F38" s="1">
         <v>12</v>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="H38" s="1">
         <f t="shared" si="3"/>
-        <v>2.987648314953902E-4</v>
+        <v>2.9876483149539022</v>
       </c>
       <c r="I38" s="1">
         <v>4</v>
@@ -3781,7 +3781,7 @@
       </c>
       <c r="K38" s="1">
         <f t="shared" si="4"/>
-        <v>9.7895515626694063E-5</v>
+        <v>0.97895515626694052</v>
       </c>
       <c r="L38" s="1">
         <v>9</v>
@@ -3791,29 +3791,29 @@
       </c>
       <c r="N38" s="1">
         <f t="shared" si="5"/>
-        <v>2.1724563432828616E-4</v>
+        <v>2.1724563432828616</v>
       </c>
       <c r="O38" s="1">
         <v>10</v>
       </c>
       <c r="P38" s="1">
+        <f t="shared" si="8"/>
+        <v>4142776</v>
+      </c>
+      <c r="Q38" s="1">
+        <f t="shared" si="6"/>
+        <v>2.4138403814254019</v>
+      </c>
+      <c r="R38" s="1">
+        <v>13</v>
+      </c>
+      <c r="S38" s="1">
         <f t="shared" si="9"/>
         <v>4142776</v>
       </c>
-      <c r="Q38" s="1">
-        <f t="shared" si="6"/>
-        <v>2.4138403814254018E-4</v>
-      </c>
-      <c r="R38" s="1">
-        <v>13</v>
-      </c>
-      <c r="S38" s="1">
-        <f t="shared" si="10"/>
-        <v>4142776</v>
-      </c>
       <c r="T38" s="1">
         <f t="shared" si="7"/>
-        <v>3.1379924958530221E-4</v>
+        <v>3.1379924958530223</v>
       </c>
       <c r="U38" s="1">
         <v>62</v>
@@ -3833,8 +3833,8 @@
         <v>12790341</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="8"/>
-        <v>8.6002398215966259E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.86002398215966247</v>
       </c>
       <c r="F39" s="1">
         <v>22</v>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="H39" s="1">
         <f t="shared" si="3"/>
-        <v>1.7199426727471331E-4</v>
+        <v>1.719942672747133</v>
       </c>
       <c r="I39" s="1">
         <v>15</v>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="K39" s="1">
         <f t="shared" si="4"/>
-        <v>1.1730585977961357E-4</v>
+        <v>1.1730585977961356</v>
       </c>
       <c r="L39" s="1">
         <v>22</v>
@@ -3864,29 +3864,29 @@
       </c>
       <c r="N39" s="1">
         <f t="shared" si="5"/>
-        <v>1.7180068278276812E-4</v>
+        <v>1.7180068278276812</v>
       </c>
       <c r="O39" s="1">
         <v>20</v>
       </c>
       <c r="P39" s="1">
+        <f t="shared" si="8"/>
+        <v>12805537</v>
+      </c>
+      <c r="Q39" s="1">
+        <f t="shared" si="6"/>
+        <v>1.5618243889342556</v>
+      </c>
+      <c r="R39" s="1">
+        <v>23</v>
+      </c>
+      <c r="S39" s="1">
         <f t="shared" si="9"/>
         <v>12805537</v>
       </c>
-      <c r="Q39" s="1">
-        <f t="shared" si="6"/>
-        <v>1.5618243889342555E-4</v>
-      </c>
-      <c r="R39" s="1">
-        <v>23</v>
-      </c>
-      <c r="S39" s="1">
-        <f t="shared" si="10"/>
-        <v>12805537</v>
-      </c>
       <c r="T39" s="1">
         <f t="shared" si="7"/>
-        <v>1.796098047274394E-4</v>
+        <v>1.7960980472743939</v>
       </c>
       <c r="U39" s="1">
         <v>113</v>
@@ -3906,8 +3906,8 @@
         <v>1054782</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" si="8"/>
-        <v>9.4806320168527717E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.94806320168527713</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="K40" s="1">
         <f t="shared" si="4"/>
-        <v>9.4556746340181125E-5</v>
+        <v>0.9455674634018113</v>
       </c>
       <c r="L40" s="1">
         <v>0</v>
@@ -3943,23 +3943,23 @@
         <v>1</v>
       </c>
       <c r="P40" s="1">
+        <f t="shared" si="8"/>
+        <v>1059639</v>
+      </c>
+      <c r="Q40" s="1">
+        <f t="shared" si="6"/>
+        <v>0.94371762458724151</v>
+      </c>
+      <c r="R40" s="1">
+        <v>2</v>
+      </c>
+      <c r="S40" s="1">
         <f t="shared" si="9"/>
         <v>1059639</v>
       </c>
-      <c r="Q40" s="1">
-        <f t="shared" si="6"/>
-        <v>9.437176245872415E-5</v>
-      </c>
-      <c r="R40" s="1">
-        <v>2</v>
-      </c>
-      <c r="S40" s="1">
-        <f t="shared" si="10"/>
-        <v>1059639</v>
-      </c>
       <c r="T40" s="1">
         <f t="shared" si="7"/>
-        <v>1.887435249174483E-4</v>
+        <v>1.887435249174483</v>
       </c>
       <c r="U40" s="1">
         <v>5</v>
@@ -3979,8 +3979,8 @@
         <v>4824758</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="8"/>
-        <v>4.1452856288336118E-4</v>
+        <f t="shared" si="2"/>
+        <v>4.1452856288336113</v>
       </c>
       <c r="F41" s="1">
         <v>12</v>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="H41" s="1">
         <f t="shared" si="3"/>
-        <v>2.4527723788396872E-4</v>
+        <v>2.4527723788396876</v>
       </c>
       <c r="I41" s="1">
         <v>3</v>
@@ -4000,7 +4000,7 @@
       </c>
       <c r="K41" s="1">
         <f t="shared" si="4"/>
-        <v>6.0486041636171619E-5</v>
+        <v>0.60486041636171617</v>
       </c>
       <c r="L41" s="1">
         <v>0</v>
@@ -4016,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="P41" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5024369</v>
       </c>
       <c r="Q41" s="1">
@@ -4027,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="S41" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>5024369</v>
       </c>
       <c r="T41" s="1">
@@ -4052,7 +4052,7 @@
         <v>849455</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F42" s="1">
@@ -4089,7 +4089,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>869666</v>
       </c>
       <c r="Q42" s="1">
@@ -4100,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="S42" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>869666</v>
       </c>
       <c r="T42" s="1">
@@ -4125,8 +4125,8 @@
         <v>6540007</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="8"/>
-        <v>3.0581007023386976E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.30581007023386975</v>
       </c>
       <c r="F43" s="1">
         <v>3</v>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="H43" s="1">
         <f t="shared" si="3"/>
-        <v>4.551850585201084E-5</v>
+        <v>0.45518505852010843</v>
       </c>
       <c r="I43" s="1">
         <v>7</v>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="K43" s="1">
         <f t="shared" si="4"/>
-        <v>1.052725928519308E-4</v>
+        <v>1.052725928519308</v>
       </c>
       <c r="L43" s="1">
         <v>6</v>
@@ -4156,29 +4156,29 @@
       </c>
       <c r="N43" s="1">
         <f t="shared" si="5"/>
-        <v>8.9339105036581381E-5</v>
+        <v>0.8933910503658139</v>
       </c>
       <c r="O43" s="1">
         <v>5</v>
       </c>
       <c r="P43" s="1">
+        <f t="shared" si="8"/>
+        <v>6715984</v>
+      </c>
+      <c r="Q43" s="1">
+        <f t="shared" si="6"/>
+        <v>0.74449254197151149</v>
+      </c>
+      <c r="R43" s="1">
+        <v>4</v>
+      </c>
+      <c r="S43" s="1">
         <f t="shared" si="9"/>
         <v>6715984</v>
       </c>
-      <c r="Q43" s="1">
-        <f t="shared" si="6"/>
-        <v>7.4449254197151153E-5</v>
-      </c>
-      <c r="R43" s="1">
-        <v>4</v>
-      </c>
-      <c r="S43" s="1">
-        <f t="shared" si="10"/>
-        <v>6715984</v>
-      </c>
       <c r="T43" s="1">
         <f t="shared" si="7"/>
-        <v>5.9559403357720925E-5</v>
+        <v>0.59559403357720919</v>
       </c>
       <c r="U43" s="1">
         <v>27</v>
@@ -4198,8 +4198,8 @@
         <v>26954436</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="8"/>
-        <v>1.1129893424592524E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.1129893424592525</v>
       </c>
       <c r="F44" s="1">
         <v>47</v>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="H44" s="1">
         <f t="shared" si="3"/>
-        <v>1.7118996695669403E-4</v>
+        <v>1.7118996695669404</v>
       </c>
       <c r="I44" s="1">
         <v>25</v>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="K44" s="1">
         <f t="shared" si="4"/>
-        <v>8.959012232348614E-5</v>
+        <v>0.89590122323486132</v>
       </c>
       <c r="L44" s="1">
         <v>31</v>
@@ -4229,29 +4229,29 @@
       </c>
       <c r="N44" s="1">
         <f t="shared" si="5"/>
-        <v>1.0952284922208394E-4</v>
+        <v>1.0952284922208395</v>
       </c>
       <c r="O44" s="1">
         <v>23</v>
       </c>
       <c r="P44" s="1">
+        <f t="shared" si="8"/>
+        <v>28304596</v>
+      </c>
+      <c r="Q44" s="1">
+        <f t="shared" si="6"/>
+        <v>0.81258888132513885</v>
+      </c>
+      <c r="R44" s="1">
+        <v>37</v>
+      </c>
+      <c r="S44" s="1">
         <f t="shared" si="9"/>
         <v>28304596</v>
       </c>
-      <c r="Q44" s="1">
-        <f t="shared" si="6"/>
-        <v>8.1258888132513889E-5</v>
-      </c>
-      <c r="R44" s="1">
-        <v>37</v>
-      </c>
-      <c r="S44" s="1">
-        <f t="shared" si="10"/>
-        <v>28304596</v>
-      </c>
       <c r="T44" s="1">
         <f t="shared" si="7"/>
-        <v>1.3072082003926145E-4</v>
+        <v>1.3072082003926146</v>
       </c>
       <c r="U44" s="1">
         <v>193</v>
@@ -4271,8 +4271,8 @@
         <v>2938671</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="8"/>
-        <v>8.8475368627519027E-4</v>
+        <f t="shared" si="2"/>
+        <v>8.8475368627519035</v>
       </c>
       <c r="F45" s="1">
         <v>3</v>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="H45" s="1">
         <f t="shared" si="3"/>
-        <v>1.0050530718274578E-4</v>
+        <v>1.0050530718274577</v>
       </c>
       <c r="I45" s="1">
         <v>14</v>
@@ -4292,7 +4292,7 @@
       </c>
       <c r="K45" s="1">
         <f t="shared" si="4"/>
-        <v>4.5987266126009708E-4</v>
+        <v>4.5987266126009709</v>
       </c>
       <c r="L45" s="1">
         <v>3</v>
@@ -4302,29 +4302,29 @@
       </c>
       <c r="N45" s="1">
         <f t="shared" si="5"/>
-        <v>9.6717005718876547E-5</v>
+        <v>0.96717005718876548</v>
       </c>
       <c r="O45" s="1">
         <v>2</v>
       </c>
       <c r="P45" s="1">
+        <f t="shared" si="8"/>
+        <v>3101833</v>
+      </c>
+      <c r="Q45" s="1">
+        <f t="shared" si="6"/>
+        <v>0.64478003812584361</v>
+      </c>
+      <c r="R45" s="1">
+        <v>3</v>
+      </c>
+      <c r="S45" s="1">
         <f t="shared" si="9"/>
         <v>3101833</v>
       </c>
-      <c r="Q45" s="1">
-        <f t="shared" si="6"/>
-        <v>6.4478003812584364E-5</v>
-      </c>
-      <c r="R45" s="1">
-        <v>3</v>
-      </c>
-      <c r="S45" s="1">
-        <f t="shared" si="10"/>
-        <v>3101833</v>
-      </c>
       <c r="T45" s="1">
         <f t="shared" si="7"/>
-        <v>9.6717005718876547E-5</v>
+        <v>0.96717005718876548</v>
       </c>
       <c r="U45" s="1">
         <v>51</v>
@@ -4344,7 +4344,7 @@
         <v>625665</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F46" s="1">
@@ -4381,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="P46" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>623657</v>
       </c>
       <c r="Q46" s="1">
@@ -4392,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="S46" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>623657</v>
       </c>
       <c r="T46" s="1">
@@ -4417,8 +4417,8 @@
         <v>8316902</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="8"/>
-        <v>1.6833191012711224E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.6833191012711224</v>
       </c>
       <c r="F47" s="1">
         <v>8</v>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="H47" s="1">
         <f t="shared" si="3"/>
-        <v>9.5616383245762668E-5</v>
+        <v>0.95616383245762659</v>
       </c>
       <c r="I47" s="1">
         <v>7</v>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="K47" s="1">
         <f t="shared" si="4"/>
-        <v>8.3190918403970354E-5</v>
+        <v>0.83190918403970349</v>
       </c>
       <c r="L47" s="1">
         <v>22</v>
@@ -4448,29 +4448,29 @@
       </c>
       <c r="N47" s="1">
         <f t="shared" si="5"/>
-        <v>2.5973964642350315E-4</v>
+        <v>2.5973964642350316</v>
       </c>
       <c r="O47" s="1">
         <v>34</v>
       </c>
       <c r="P47" s="1">
+        <f t="shared" si="8"/>
+        <v>8470020</v>
+      </c>
+      <c r="Q47" s="1">
+        <f t="shared" si="6"/>
+        <v>4.0141581719995942</v>
+      </c>
+      <c r="R47" s="1">
+        <v>38</v>
+      </c>
+      <c r="S47" s="1">
         <f t="shared" si="9"/>
         <v>8470020</v>
       </c>
-      <c r="Q47" s="1">
-        <f t="shared" si="6"/>
-        <v>4.0141581719995941E-4</v>
-      </c>
-      <c r="R47" s="1">
-        <v>38</v>
-      </c>
-      <c r="S47" s="1">
-        <f t="shared" si="10"/>
-        <v>8470020</v>
-      </c>
       <c r="T47" s="1">
         <f t="shared" si="7"/>
-        <v>4.4864120745877808E-4</v>
+        <v>4.4864120745877809</v>
       </c>
       <c r="U47" s="1">
         <v>123</v>
@@ -4490,8 +4490,8 @@
         <v>7046931</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="8"/>
-        <v>1.2771517132777375E-4</v>
+        <f t="shared" si="2"/>
+        <v>1.2771517132777375</v>
       </c>
       <c r="F48" s="1">
         <v>14</v>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="H48" s="1">
         <f t="shared" si="3"/>
-        <v>1.9572705470766906E-4</v>
+        <v>1.9572705470766907</v>
       </c>
       <c r="I48" s="1">
         <v>12</v>
@@ -4511,7 +4511,7 @@
       </c>
       <c r="K48" s="1">
         <f t="shared" si="4"/>
-        <v>1.6481401973977513E-4</v>
+        <v>1.6481401973977514</v>
       </c>
       <c r="L48" s="1">
         <v>9</v>
@@ -4521,29 +4521,29 @@
       </c>
       <c r="N48" s="1">
         <f t="shared" si="5"/>
-        <v>1.2152730657815158E-4</v>
+        <v>1.2152730657815158</v>
       </c>
       <c r="O48" s="1">
         <v>6</v>
       </c>
       <c r="P48" s="1">
+        <f t="shared" si="8"/>
+        <v>7405743</v>
+      </c>
+      <c r="Q48" s="1">
+        <f t="shared" si="6"/>
+        <v>0.81018204385434389</v>
+      </c>
+      <c r="R48" s="1">
+        <v>9</v>
+      </c>
+      <c r="S48" s="1">
         <f t="shared" si="9"/>
         <v>7405743</v>
       </c>
-      <c r="Q48" s="1">
-        <f t="shared" si="6"/>
-        <v>8.1018204385434388E-5</v>
-      </c>
-      <c r="R48" s="1">
-        <v>9</v>
-      </c>
-      <c r="S48" s="1">
-        <f t="shared" si="10"/>
-        <v>7405743</v>
-      </c>
       <c r="T48" s="1">
         <f t="shared" si="7"/>
-        <v>1.2152730657815158E-4</v>
+        <v>1.2152730657815158</v>
       </c>
       <c r="U48" s="1">
         <v>59</v>
@@ -4563,7 +4563,7 @@
         <v>1847624</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F49" s="1">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="H49" s="1">
         <f t="shared" si="3"/>
-        <v>5.4354709047395676E-5</v>
+        <v>0.54354709047395677</v>
       </c>
       <c r="I49" s="1">
         <v>0</v>
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1815857</v>
       </c>
       <c r="Q49" s="1">
@@ -4611,7 +4611,7 @@
         <v>0</v>
       </c>
       <c r="S49" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1815857</v>
       </c>
       <c r="T49" s="1">
@@ -4636,8 +4636,8 @@
         <v>5751272</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" si="8"/>
-        <v>6.9549831758956978E-5</v>
+        <f t="shared" si="2"/>
+        <v>0.6954983175895697</v>
       </c>
       <c r="F50" s="1">
         <v>5</v>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="H50" s="1">
         <f t="shared" si="3"/>
-        <v>8.6809413751722298E-5</v>
+        <v>0.86809413751722297</v>
       </c>
       <c r="I50" s="1">
         <v>3</v>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="K50" s="1">
         <f t="shared" si="4"/>
-        <v>5.1966795988925533E-5</v>
+        <v>0.51966795988925529</v>
       </c>
       <c r="L50" s="1">
         <v>7</v>
@@ -4667,29 +4667,29 @@
       </c>
       <c r="N50" s="1">
         <f t="shared" si="5"/>
-        <v>1.2078372070110464E-4</v>
+        <v>1.2078372070110464</v>
       </c>
       <c r="O50" s="1">
         <v>4</v>
       </c>
       <c r="P50" s="1">
+        <f t="shared" si="8"/>
+        <v>5795483</v>
+      </c>
+      <c r="Q50" s="1">
+        <f t="shared" si="6"/>
+        <v>0.690192689720598</v>
+      </c>
+      <c r="R50" s="1">
+        <v>10</v>
+      </c>
+      <c r="S50" s="1">
         <f t="shared" si="9"/>
         <v>5795483</v>
       </c>
-      <c r="Q50" s="1">
-        <f t="shared" si="6"/>
-        <v>6.9019268972059792E-5</v>
-      </c>
-      <c r="R50" s="1">
-        <v>10</v>
-      </c>
-      <c r="S50" s="1">
-        <f t="shared" si="10"/>
-        <v>5795483</v>
-      </c>
       <c r="T50" s="1">
         <f t="shared" si="7"/>
-        <v>1.7254817243014949E-4</v>
+        <v>1.7254817243014948</v>
       </c>
       <c r="U50" s="1">
         <v>33</v>
@@ -4709,7 +4709,7 @@
         <v>583334</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F51" s="1">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="K51" s="1">
         <f t="shared" si="4"/>
-        <v>3.4193294694910326E-4</v>
+        <v>3.4193294694910326</v>
       </c>
       <c r="L51" s="1">
         <v>1</v>
@@ -4740,28 +4740,28 @@
       </c>
       <c r="N51" s="1">
         <f t="shared" si="5"/>
-        <v>1.7261766051284707E-4</v>
+        <v>1.7261766051284708</v>
       </c>
       <c r="O51" s="1">
         <v>0</v>
       </c>
       <c r="P51" s="1">
+        <f t="shared" si="8"/>
+        <v>579315</v>
+      </c>
+      <c r="Q51" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R51" s="1">
+        <v>0</v>
+      </c>
+      <c r="S51" s="1">
         <f t="shared" si="9"/>
         <v>579315</v>
       </c>
-      <c r="Q51" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R51" s="1">
-        <v>0</v>
-      </c>
-      <c r="S51" s="1">
-        <f t="shared" si="10"/>
-        <v>579315</v>
-      </c>
       <c r="T51" s="1">
-        <f ca="1">C1:T51=(R51/S51)*100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U51" s="1">

</xml_diff>